<commit_message>
Updated everything post-week 12
</commit_message>
<xml_diff>
--- a/live-pts.xlsx
+++ b/live-pts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dwyerry/programming/fantasy-playoffs-w13/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDFDCAC-70B9-5E42-890C-B7E1289922BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8FC1B8-26AB-484B-BE2E-218571A601D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15360" yWindow="460" windowWidth="15360" windowHeight="18740" xr2:uid="{40AE0D34-C8D7-B846-A940-F620CC1B2841}"/>
   </bookViews>
@@ -456,7 +456,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -477,10 +477,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>105.78</v>
+        <v>112.78</v>
       </c>
       <c r="C2">
-        <v>112.44</v>
+        <v>112.78</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -554,10 +554,10 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>94.1</v>
+        <v>104.84</v>
       </c>
       <c r="C9">
-        <v>105.3</v>
+        <v>104.84</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -576,10 +576,10 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>144.63999999999999</v>
+        <v>147.74</v>
       </c>
       <c r="C11">
-        <v>147.55000000000001</v>
+        <v>147.74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>